<commit_message>
Create prediction files for 5 years.
</commit_message>
<xml_diff>
--- a/Settings/NN_setting.xlsx
+++ b/Settings/NN_setting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nauka\GitHub\cge_model_python\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F7E58F-5CD1-4505-8617-1D4E913C5C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3254FD2-A17E-4335-9784-05F3B41E3E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="4860" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>households</t>
-  </si>
-  <si>
-    <t>government</t>
   </si>
   <si>
     <t>factors</t>
@@ -522,23 +519,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,203 +548,200 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>